<commit_message>
Commit 3b since earlier was misnumbered
</commit_message>
<xml_diff>
--- a/Resources/data dictionary.xlsx
+++ b/Resources/data dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://communsol-my.sharepoint.com/personal/judith_calvo_communitysolutions_org/Documents/_aUCB Data Analytics Bootcamp Class/Final Project Folder/ML/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{B21A9620-161B-4566-BA0D-1C5DCEAAAA5F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{6929B8B5-101D-4378-8D1F-5367FE60CA9B}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{B21A9620-161B-4566-BA0D-1C5DCEAAAA5F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D927847B-8BB5-44DE-9A1B-D370D7111B4E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{DE68D33D-2361-456F-8777-3D3631C620A9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="5" xr2:uid="{DE68D33D-2361-456F-8777-3D3631C620A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="analysis data with dummy vars" sheetId="3" r:id="rId3"/>
     <sheet name="first logistic regression model" sheetId="4" r:id="rId4"/>
     <sheet name="second logistic regression mode" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
+    <sheet name="third model" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="189">
   <si>
     <t>EPISODE_NUMBER</t>
   </si>
@@ -573,6 +573,36 @@
   </si>
   <si>
     <t>Confidence Interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Current function value: 0.608731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Iterations 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                 Results: Logit</t>
+  </si>
+  <si>
+    <t>================================================================================================================================================</t>
+  </si>
+  <si>
+    <t>Dependent Variable:</t>
+  </si>
+  <si>
+    <t>No. Observations:</t>
+  </si>
+  <si>
+    <t>Df Model:</t>
+  </si>
+  <si>
+    <t>Df Residuals:</t>
+  </si>
+  <si>
+    <t>LLR p-value:</t>
+  </si>
+  <si>
+    <t>No. Iterations:</t>
   </si>
 </sst>
 </file>
@@ -580,7 +610,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -695,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -731,7 +761,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,8 +802,8 @@
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>2413000</xdr:colOff>
-          <xdr:row>47</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -778,7 +813,7 @@
                   <a14:compatExt spid="_x0000_s5121"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{249EEDBC-FA6B-4654-A099-574326E9815F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001140000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3386,7 +3421,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -4191,8 +4226,8 @@
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>2413000</xdr:colOff>
-                <xdr:row>47</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
+                <xdr:row>48</xdr:row>
+                <xdr:rowOff>6350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -4207,33 +4242,763 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8DD44F-EF87-41CD-8893-2A52101A1363}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B1DCEC-8084-49B0-B709-E60E28DB5651}">
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="22">
+        <v>1586.8731</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="22">
+        <v>1710.2819999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9">
+        <v>1264</v>
+      </c>
+      <c r="D9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="22">
+        <v>-769.44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="22">
+        <v>-857.59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11">
+        <v>1240</v>
+      </c>
+      <c r="D11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="22">
+        <v>1.3143999999999999E-25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>0.02</v>
+      </c>
+      <c r="C17">
+        <v>0.13439999999999999</v>
+      </c>
+      <c r="D17">
+        <v>0.14910000000000001</v>
+      </c>
+      <c r="E17" s="22">
+        <v>0.88149999999999995</v>
+      </c>
+      <c r="F17">
+        <v>-0.24340000000000001</v>
+      </c>
+      <c r="G17">
+        <v>0.28339999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="17">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="C18" s="17">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D18" s="17">
+        <v>9.5327000000000002</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+      <c r="F18" s="17">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="G18" s="17">
+        <v>5.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="17">
+        <v>0.15060000000000001</v>
+      </c>
+      <c r="C19" s="17">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="D19" s="17">
+        <v>1.7312000000000001</v>
+      </c>
+      <c r="E19" s="24">
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="F19" s="17">
+        <v>-1.9900000000000001E-2</v>
+      </c>
+      <c r="G19" s="17">
+        <v>0.3211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>-0.1139</v>
+      </c>
+      <c r="C20">
+        <v>0.1095</v>
+      </c>
+      <c r="D20">
+        <v>-1.0401</v>
+      </c>
+      <c r="E20" s="22">
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="F20">
+        <v>-0.32850000000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.1007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>-0.1042</v>
+      </c>
+      <c r="C21">
+        <v>8.7400000000000005E-2</v>
+      </c>
+      <c r="D21">
+        <v>-1.1917</v>
+      </c>
+      <c r="E21" s="22">
+        <v>0.2334</v>
+      </c>
+      <c r="F21">
+        <v>-0.27539999999999998</v>
+      </c>
+      <c r="G21">
+        <v>6.7100000000000007E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>-6.4399999999999999E-2</v>
+      </c>
+      <c r="C22">
+        <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="D22">
+        <v>-0.76160000000000005</v>
+      </c>
+      <c r="E22" s="22">
+        <v>0.44629999999999997</v>
+      </c>
+      <c r="F22">
+        <v>-0.2301</v>
+      </c>
+      <c r="G22">
+        <v>0.1013</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="17">
+        <v>-0.36599999999999999</v>
+      </c>
+      <c r="C23" s="17">
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="D23" s="17">
+        <v>-3.7542</v>
+      </c>
+      <c r="E23" s="24">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F23" s="17">
+        <v>-0.55710000000000004</v>
+      </c>
+      <c r="G23" s="17">
+        <v>-0.1749</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>0.14449999999999999</v>
+      </c>
+      <c r="C24">
+        <v>0.15279999999999999</v>
+      </c>
+      <c r="D24">
+        <v>0.94540000000000002</v>
+      </c>
+      <c r="E24" s="22">
+        <v>0.34449999999999997</v>
+      </c>
+      <c r="F24">
+        <v>-0.15509999999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.44409999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>-0.1128</v>
+      </c>
+      <c r="C25">
+        <v>0.1241</v>
+      </c>
+      <c r="D25">
+        <v>-0.9093</v>
+      </c>
+      <c r="E25" s="22">
+        <v>0.36320000000000002</v>
+      </c>
+      <c r="F25">
+        <v>-0.35599999999999998</v>
+      </c>
+      <c r="G25">
+        <v>0.13039999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>-4.19E-2</v>
+      </c>
+      <c r="C26">
+        <v>8.6699999999999999E-2</v>
+      </c>
+      <c r="D26">
+        <v>-0.4834</v>
+      </c>
+      <c r="E26" s="22">
+        <v>0.62880000000000003</v>
+      </c>
+      <c r="F26">
+        <v>-0.2117</v>
+      </c>
+      <c r="G26">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="C27">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D27">
+        <v>0.7611</v>
+      </c>
+      <c r="E27" s="22">
+        <v>0.4466</v>
+      </c>
+      <c r="F27">
+        <v>-4.19E-2</v>
+      </c>
+      <c r="G27">
+        <v>9.5100000000000004E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="17">
+        <v>-6.1699999999999998E-2</v>
+      </c>
+      <c r="C28" s="17">
+        <v>1.83E-2</v>
+      </c>
+      <c r="D28" s="17">
+        <v>-3.3668</v>
+      </c>
+      <c r="E28" s="24">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="F28" s="17">
+        <v>-9.7600000000000006E-2</v>
+      </c>
+      <c r="G28" s="17">
+        <v>-2.58E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="17">
+        <v>0.26329999999999998</v>
+      </c>
+      <c r="C29" s="17">
+        <v>8.8099999999999998E-2</v>
+      </c>
+      <c r="D29" s="17">
+        <v>2.9876</v>
+      </c>
+      <c r="E29" s="24">
+        <v>2.8E-3</v>
+      </c>
+      <c r="F29" s="17">
+        <v>9.06E-2</v>
+      </c>
+      <c r="G29" s="17">
+        <v>0.43609999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30">
+        <v>2.86E-2</v>
+      </c>
+      <c r="C30">
+        <v>8469056.9065000005</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" s="22">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>-16599046.4911</v>
+      </c>
+      <c r="G30">
+        <v>16599046.5483</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31">
+        <v>-0.20150000000000001</v>
+      </c>
+      <c r="C31">
+        <v>8469056.9065000005</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="22">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>-16599046.7213</v>
+      </c>
+      <c r="G31">
+        <v>16599046.3182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32">
+        <v>-1.9099999999999999E-2</v>
+      </c>
+      <c r="C32">
+        <v>8469056.9065000005</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="22">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>-16599046.538899999</v>
+      </c>
+      <c r="G32">
+        <v>16599046.500600001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33">
+        <v>-4.8500000000000001E-2</v>
+      </c>
+      <c r="C33">
+        <v>8469056.9065000005</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="22">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>-16599046.5682</v>
+      </c>
+      <c r="G33">
+        <v>16599046.4712</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34">
+        <v>-0.1153</v>
+      </c>
+      <c r="C34">
+        <v>8469056.9065000005</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" s="22">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>-16599046.635</v>
+      </c>
+      <c r="G34">
+        <v>16599046.4044</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35">
+        <v>-2.8199999999999999E-2</v>
+      </c>
+      <c r="C35">
+        <v>8469056.9065000005</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" s="22">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>-16599046.547900001</v>
+      </c>
+      <c r="G35">
+        <v>16599046.4915</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36">
+        <v>-0.59309999999999996</v>
+      </c>
+      <c r="C36">
+        <v>0.31759999999999999</v>
+      </c>
+      <c r="D36">
+        <v>-1.8673</v>
+      </c>
+      <c r="E36" s="22">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="F36">
+        <v>-1.2156</v>
+      </c>
+      <c r="G36">
+        <v>2.9399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37">
+        <v>-0.184</v>
+      </c>
+      <c r="C37">
+        <v>0.27450000000000002</v>
+      </c>
+      <c r="D37">
+        <v>-0.67010000000000003</v>
+      </c>
+      <c r="E37" s="22">
+        <v>0.50280000000000002</v>
+      </c>
+      <c r="F37">
+        <v>-0.72199999999999998</v>
+      </c>
+      <c r="G37">
+        <v>0.35410000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38">
+        <v>-0.65629999999999999</v>
+      </c>
+      <c r="C38">
+        <v>0.2878</v>
+      </c>
+      <c r="D38">
+        <v>-2.2801</v>
+      </c>
+      <c r="E38" s="22">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="F38">
+        <v>-1.2204999999999999</v>
+      </c>
+      <c r="G38">
+        <v>-9.2100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="C39">
+        <v>0.17050000000000001</v>
+      </c>
+      <c r="D39">
+        <v>-0.41049999999999998</v>
+      </c>
+      <c r="E39" s="22">
+        <v>0.68140000000000001</v>
+      </c>
+      <c r="F39">
+        <v>-0.4042</v>
+      </c>
+      <c r="G39">
+        <v>0.26419999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B40">
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="C40">
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="D40">
+        <v>0.25629999999999997</v>
+      </c>
+      <c r="E40" s="22">
+        <v>0.79769999999999996</v>
+      </c>
+      <c r="F40">
+        <v>-0.48980000000000001</v>
+      </c>
+      <c r="G40">
+        <v>0.63719999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41">
+        <v>0.13769999999999999</v>
+      </c>
+      <c r="C41">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="D41">
+        <v>0.4652</v>
+      </c>
+      <c r="E41" s="22">
+        <v>0.64180000000000004</v>
+      </c>
+      <c r="F41">
+        <v>-0.44240000000000002</v>
+      </c>
+      <c r="G41">
+        <v>0.71779999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B03C3E295CF76648AC85B6EC26361ECA" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0bb9dd14d241c245318bb8942e244b1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b42430d8-c205-408e-a6b2-f7bcf1ddda46" xmlns:ns4="076ed714-3a77-4f17-8bbf-04471c3fc2e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d56a7a2c73efd02ab063fa24f087166" ns3:_="" ns4:_="">
     <xsd:import namespace="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
@@ -4456,32 +5221,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{571F5220-80D8-4F20-8AD7-DC1A6F626947}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78112817-9362-4DB1-B53E-54BAB126672D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ABF22CB-D5B7-49AE-88C0-4633C565A5F4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4498,4 +5253,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78112817-9362-4DB1-B53E-54BAB126672D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{571F5220-80D8-4F20-8AD7-DC1A6F626947}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commit 5 for the two week period up to June 14th
</commit_message>
<xml_diff>
--- a/Resources/data dictionary.xlsx
+++ b/Resources/data dictionary.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="137" documentId="8_{B21A9620-161B-4566-BA0D-1C5DCEAAAA5F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D927847B-8BB5-44DE-9A1B-D370D7111B4E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="5" xr2:uid="{DE68D33D-2361-456F-8777-3D3631C620A9}"/>
+    <workbookView xWindow="23904" yWindow="864" windowWidth="17280" windowHeight="8916" firstSheet="4" activeTab="5" xr2:uid="{DE68D33D-2361-456F-8777-3D3631C620A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -796,14 +796,14 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>43</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>41</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2413000</xdr:colOff>
-          <xdr:row>48</xdr:row>
-          <xdr:rowOff>6350</xdr:rowOff>
+          <xdr:colOff>2787650</xdr:colOff>
+          <xdr:row>47</xdr:row>
+          <xdr:rowOff>17780</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4220,14 +4220,14 @@
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>43</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>165100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>2413000</xdr:colOff>
-                <xdr:row>48</xdr:row>
-                <xdr:rowOff>6350</xdr:rowOff>
+                <xdr:colOff>2787650</xdr:colOff>
+                <xdr:row>47</xdr:row>
+                <xdr:rowOff>25400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -4999,6 +4999,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B03C3E295CF76648AC85B6EC26361ECA" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0bb9dd14d241c245318bb8942e244b1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b42430d8-c205-408e-a6b2-f7bcf1ddda46" xmlns:ns4="076ed714-3a77-4f17-8bbf-04471c3fc2e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d56a7a2c73efd02ab063fa24f087166" ns3:_="" ns4:_="">
     <xsd:import namespace="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
@@ -5221,7 +5227,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5230,13 +5236,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{571F5220-80D8-4F20-8AD7-DC1A6F626947}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ABF22CB-D5B7-49AE-88C0-4633C565A5F4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5255,27 +5272,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78112817-9362-4DB1-B53E-54BAB126672D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{571F5220-80D8-4F20-8AD7-DC1A6F626947}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commit for June 11 2020
</commit_message>
<xml_diff>
--- a/Resources/data dictionary.xlsx
+++ b/Resources/data dictionary.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://communsol-my.sharepoint.com/personal/judith_calvo_communitysolutions_org/Documents/_aUCB Data Analytics Bootcamp Class/Final Project Folder/ML/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{B21A9620-161B-4566-BA0D-1C5DCEAAAA5F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D927847B-8BB5-44DE-9A1B-D370D7111B4E}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="8_{B21A9620-161B-4566-BA0D-1C5DCEAAAA5F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{51654E9D-7529-4475-8685-0D16D8B5B5F7}"/>
   <bookViews>
-    <workbookView xWindow="23904" yWindow="864" windowWidth="17280" windowHeight="8916" firstSheet="4" activeTab="5" xr2:uid="{DE68D33D-2361-456F-8777-3D3631C620A9}"/>
+    <workbookView xWindow="950" yWindow="720" windowWidth="17280" windowHeight="8920" firstSheet="3" activeTab="5" xr2:uid="{DE68D33D-2361-456F-8777-3D3631C620A9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="original data set for database" sheetId="1" r:id="rId1"/>
     <sheet name="final data types" sheetId="2" r:id="rId2"/>
-    <sheet name="analysis data with dummy vars" sheetId="3" r:id="rId3"/>
+    <sheet name="variables with dummies" sheetId="3" r:id="rId3"/>
     <sheet name="first logistic regression model" sheetId="4" r:id="rId4"/>
     <sheet name="second logistic regression mode" sheetId="5" r:id="rId5"/>
     <sheet name="third model" sheetId="7" r:id="rId6"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="181">
   <si>
     <t>EPISODE_NUMBER</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Data Type</t>
   </si>
   <si>
-    <t>['patient_sex_code',</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 'length_of_stay',</t>
   </si>
   <si>
@@ -335,12 +332,6 @@
     <t xml:space="preserve"> 'diagnosis_value_Posttraumatic stress disorder',</t>
   </si>
   <si>
-    <t xml:space="preserve"> 'diagnosis_value_Unspecified anxiety disorder']</t>
-  </si>
-  <si>
-    <t>patient</t>
-  </si>
-  <si>
     <t>import statsmodels.api as sm</t>
   </si>
   <si>
@@ -365,33 +356,6 @@
     <t xml:space="preserve">                                                                Results: Logit</t>
   </si>
   <si>
-    <t>==============================================================================================================================================</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model:                                         Logit                                     Pseudo R-squared:                          0.119     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dependent Variable:                            y                                         AIC:                                       1582.3906 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date:                                          2020-06-05 16:17                          BIC:                                       1767.5039 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">No. Observations:                              1264                                      Log-Likelihood:                            -755.20   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Df Model:                                      35                                        LL-Null:                                   -857.59   </t>
-  </si>
-  <si>
-    <t>Df Residuals:                                  1228                                      LLR p-value:                               6.9553e-26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Converged:                                     0.0000                                    Scale:                                     1.0000    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">No. Iterations:                                35.0000                                                                                        </t>
-  </si>
-  <si>
     <t>Coef.</t>
   </si>
   <si>
@@ -497,9 +461,6 @@
     <t>diagnosis_value_Unspecified anxiety disorder</t>
   </si>
   <si>
-    <t>Index</t>
-  </si>
-  <si>
     <t>Optimization terminated successfully.</t>
   </si>
   <si>
@@ -584,9 +545,6 @@
     <t xml:space="preserve">                                                                 Results: Logit</t>
   </si>
   <si>
-    <t>================================================================================================================================================</t>
-  </si>
-  <si>
     <t>Dependent Variable:</t>
   </si>
   <si>
@@ -603,6 +561,24 @@
   </si>
   <si>
     <t>No. Iterations:</t>
+  </si>
+  <si>
+    <t>Dummy Variables</t>
+  </si>
+  <si>
+    <t>patient_sex_code',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'diagnosis_value_Unspecified anxiety disorder'</t>
+  </si>
+  <si>
+    <t>Pseudo R-squared:</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Statistically Significant Features</t>
   </si>
 </sst>
 </file>
@@ -612,7 +588,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,6 +659,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -725,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -767,6 +750,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,13 +796,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>41</xdr:row>
-          <xdr:rowOff>167640</xdr:rowOff>
+          <xdr:rowOff>165100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>2787650</xdr:colOff>
           <xdr:row>47</xdr:row>
-          <xdr:rowOff>17780</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1143,7 +1142,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1620,10 +1619,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E335C8B6-51F3-456F-9770-7A5CF3C586F3}">
-  <dimension ref="A1:A47"/>
+  <dimension ref="A1:A45"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1632,223 +1631,226 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>57</v>
+      <c r="A1" s="26" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
-        <v>73</v>
+      <c r="A16" s="9"/>
+    </row>
+    <row r="17" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="9" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1858,40 +1860,42 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9863F624-3CCD-4F16-9563-126C489556E1}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="B1:L66"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="63.81640625" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1906,7 +1910,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1921,7 +1925,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1936,7 +1940,7 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1950,9 +1954,7 @@
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="B12" s="11"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1966,11 +1968,17 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+        <v>148</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.11899999999999999</v>
+      </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -1981,11 +1989,17 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+        <v>169</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1582.3905999999999</v>
+      </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -1996,11 +2010,17 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+        <v>179</v>
+      </c>
+      <c r="C15" s="27">
+        <v>43987.678472222222</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1767.5038999999999</v>
+      </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -2011,11 +2031,17 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+        <v>170</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1264</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="8">
+        <v>-755.2</v>
+      </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -2024,13 +2050,19 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+        <v>171</v>
+      </c>
+      <c r="C17" s="8">
+        <v>35</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="8">
+        <v>-857.59</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -2039,13 +2071,19 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+        <v>172</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1228</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" s="28">
+        <v>6.9552999999999995E-26</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -2054,13 +2092,19 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+        <v>163</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -2069,11 +2113,13 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="8"/>
+        <v>174</v>
+      </c>
+      <c r="C20" s="8">
+        <v>35</v>
+      </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -2084,7 +2130,7 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="11"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2097,35 +2143,32 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="11"/>
       <c r="C22" s="8" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>153</v>
-      </c>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="11"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2138,10 +2181,7 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>0</v>
-      </c>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="11" t="s">
         <v>31</v>
       </c>
@@ -2168,10 +2208,7 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>1</v>
-      </c>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="11" t="s">
         <v>12</v>
       </c>
@@ -2198,10 +2235,7 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>2</v>
-      </c>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="12" t="s">
         <v>47</v>
       </c>
@@ -2228,10 +2262,7 @@
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>3</v>
-      </c>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="11" t="s">
         <v>19</v>
       </c>
@@ -2258,10 +2289,7 @@
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>4</v>
-      </c>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
         <v>20</v>
       </c>
@@ -2288,10 +2316,7 @@
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>5</v>
-      </c>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" s="11" t="s">
         <v>21</v>
       </c>
@@ -2318,10 +2343,7 @@
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>6</v>
-      </c>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="11" t="s">
         <v>22</v>
       </c>
@@ -2348,10 +2370,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>7</v>
-      </c>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="12" t="s">
         <v>23</v>
       </c>
@@ -2378,10 +2397,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>8</v>
-      </c>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="11" t="s">
         <v>24</v>
       </c>
@@ -2408,10 +2424,7 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>9</v>
-      </c>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B33" s="11" t="s">
         <v>25</v>
       </c>
@@ -2438,10 +2451,7 @@
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>10</v>
-      </c>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B34" s="11" t="s">
         <v>26</v>
       </c>
@@ -2468,10 +2478,7 @@
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>11</v>
-      </c>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B35" s="12" t="s">
         <v>52</v>
       </c>
@@ -2498,10 +2505,7 @@
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>12</v>
-      </c>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B36" s="12" t="s">
         <v>53</v>
       </c>
@@ -2528,10 +2532,7 @@
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>13</v>
-      </c>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B37" s="12" t="s">
         <v>54</v>
       </c>
@@ -2558,102 +2559,90 @@
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>14</v>
-      </c>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B38" s="11" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C38" s="8">
         <v>0.59160000000000001</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>15</v>
-      </c>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B39" s="11" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C39" s="8">
         <v>0.42270000000000002</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>16</v>
-      </c>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B40" s="11" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C40" s="8">
         <v>0.2452</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>17</v>
-      </c>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B41" s="11" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C41" s="8">
         <v>0.42620000000000002</v>
@@ -2678,12 +2667,9 @@
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>18</v>
-      </c>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B42" s="11" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C42" s="8">
         <v>0.16930000000000001</v>
@@ -2708,12 +2694,9 @@
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>19</v>
-      </c>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B43" s="11" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C43" s="8">
         <v>-1.1599999999999999E-2</v>
@@ -2738,12 +2721,9 @@
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>20</v>
-      </c>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B44" s="11" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C44" s="8">
         <v>0.67559999999999998</v>
@@ -2768,102 +2748,90 @@
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>21</v>
-      </c>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B45" s="11" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C45" s="8">
         <v>-2.9386999999999999</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>22</v>
-      </c>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B46" s="11" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C46" s="8">
         <v>6.7080000000000002</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <v>23</v>
-      </c>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B47" s="11" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C47" s="8">
         <v>-2.5097</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>24</v>
-      </c>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B48" s="11" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C48" s="8">
         <v>0.5837</v>
@@ -2888,12 +2856,9 @@
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>25</v>
-      </c>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B49" s="11" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C49" s="8">
         <v>0.67589999999999995</v>
@@ -2918,102 +2883,90 @@
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>26</v>
-      </c>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B50" s="11" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C50" s="8">
         <v>0.53310000000000002</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>27</v>
-      </c>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B51" s="11" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C51" s="8">
         <v>0.25</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>28</v>
-      </c>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B52" s="11" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C52" s="8">
         <v>0.47649999999999998</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>29</v>
-      </c>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B53" s="11" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C53" s="8">
         <v>0.45710000000000001</v>
@@ -3038,12 +2991,9 @@
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <v>30</v>
-      </c>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B54" s="11" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C54" s="8">
         <v>0.36359999999999998</v>
@@ -3068,12 +3018,9 @@
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>31</v>
-      </c>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B55" s="11" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C55" s="8">
         <v>0.43890000000000001</v>
@@ -3098,307 +3045,277 @@
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>32</v>
-      </c>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B56" s="11" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C56" s="8">
         <v>0.69550000000000001</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>33</v>
-      </c>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B57" s="11" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C57" s="8">
         <v>0.1129</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>34</v>
-      </c>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B58" s="11" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C58" s="8">
         <v>-0.35630000000000001</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>35</v>
-      </c>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B59" s="11" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C59" s="8">
         <v>0.105</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I59" s="8"/>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>36</v>
-      </c>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B60" s="11" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C60" s="8">
         <v>-0.33100000000000002</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
       <c r="L60" s="8"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>37</v>
-      </c>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B61" s="11" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C61" s="8">
         <v>0.41449999999999998</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I61" s="8"/>
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>38</v>
-      </c>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B62" s="11" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C62" s="8">
         <v>-0.3574</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>39</v>
-      </c>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B63" s="11" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C63" s="8">
         <v>0.1986</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>40</v>
-      </c>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B64" s="11" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C64" s="8">
         <v>0.3201</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>41</v>
-      </c>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B65" s="11" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C65" s="8">
         <v>0.45760000000000001</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I65" s="8"/>
       <c r="J65" s="8"/>
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B66" s="11"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
@@ -3434,41 +3351,41 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E6">
         <v>0.107</v>
@@ -3476,13 +3393,13 @@
     </row>
     <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="E7">
         <v>1581.9074000000001</v>
@@ -3493,7 +3410,7 @@
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E8">
         <v>1710.4583</v>
@@ -3501,16 +3418,16 @@
     </row>
     <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="C9">
         <v>1264</v>
       </c>
       <c r="D9" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="E9">
         <v>-765.95</v>
@@ -3518,16 +3435,16 @@
     </row>
     <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C10">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="E10">
         <v>-857.59</v>
@@ -3535,19 +3452,19 @@
     </row>
     <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="C11">
         <v>1239</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="E11" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="F11" s="20">
         <v>1.7326E-26</v>
@@ -3555,13 +3472,13 @@
     </row>
     <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -3569,36 +3486,36 @@
     </row>
     <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="F14" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E15" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G15" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -3928,145 +3845,145 @@
     </row>
     <row r="31" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B31">
         <v>-2.01E-2</v>
       </c>
       <c r="C31" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E31" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G31" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B32">
         <v>-0.2626</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E32" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F32" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G32" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B33">
         <v>-6.9599999999999995E-2</v>
       </c>
       <c r="C33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B34">
         <v>-0.1018</v>
       </c>
       <c r="C34" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E34" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F34" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G34" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B35">
         <v>-0.1482</v>
       </c>
       <c r="C35" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E35" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F35" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G35" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B36">
         <v>-0.1022</v>
       </c>
       <c r="C36" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E36" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F36" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G36" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B37">
         <v>-0.59760000000000002</v>
@@ -4089,7 +4006,7 @@
     </row>
     <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B38">
         <v>-0.18260000000000001</v>
@@ -4112,7 +4029,7 @@
     </row>
     <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B39">
         <v>-0.63519999999999999</v>
@@ -4135,7 +4052,7 @@
     </row>
     <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B40">
         <v>-5.2499999999999998E-2</v>
@@ -4158,7 +4075,7 @@
     </row>
     <row r="41" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="B41">
         <v>0.1172</v>
@@ -4181,7 +4098,7 @@
     </row>
     <row r="42" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B42">
         <v>0.1661</v>
@@ -4204,7 +4121,7 @@
     </row>
     <row r="43" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -4227,7 +4144,7 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>2787650</xdr:colOff>
                 <xdr:row>47</xdr:row>
-                <xdr:rowOff>25400</xdr:rowOff>
+                <xdr:rowOff>12700</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -4246,12 +4163,12 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.81640625" customWidth="1"/>
+    <col min="1" max="1" width="64.81640625" customWidth="1"/>
     <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="22"/>
@@ -4259,22 +4176,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -4282,16 +4199,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E6" s="22">
         <v>0.10299999999999999</v>
@@ -4299,13 +4216,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="E7" s="22">
         <v>1586.8731</v>
@@ -4316,7 +4233,7 @@
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E8" s="22">
         <v>1710.2819999999999</v>
@@ -4324,13 +4241,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B9">
         <v>1264</v>
       </c>
       <c r="D9" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="E9" s="22">
         <v>-769.44</v>
@@ -4338,13 +4255,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B10">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="E10" s="22">
         <v>-857.59</v>
@@ -4352,13 +4269,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B11">
         <v>1240</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="E11" s="22">
         <v>1.3143999999999999E-25</v>
@@ -4366,13 +4283,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E12" s="22">
         <v>1</v>
@@ -4380,34 +4297,36 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
+    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="29" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G15" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -4460,25 +4379,25 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="31">
         <v>0.15060000000000001</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="31">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="31">
         <v>1.7312000000000001</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="32">
         <v>8.3400000000000002E-2</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="31">
         <v>-1.9900000000000001E-2</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="31">
         <v>0.3211</v>
       </c>
     </row>
@@ -4714,7 +4633,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B30">
         <v>2.86E-2</v>
@@ -4737,7 +4656,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B31">
         <v>-0.20150000000000001</v>
@@ -4760,7 +4679,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B32">
         <v>-1.9099999999999999E-2</v>
@@ -4783,7 +4702,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B33">
         <v>-4.8500000000000001E-2</v>
@@ -4806,7 +4725,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B34">
         <v>-0.1153</v>
@@ -4829,7 +4748,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B35">
         <v>-2.8199999999999999E-2</v>
@@ -4852,7 +4771,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B36">
         <v>-0.59309999999999996</v>
@@ -4875,7 +4794,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B37">
         <v>-0.184</v>
@@ -4898,7 +4817,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B38">
         <v>-0.65629999999999999</v>
@@ -4921,7 +4840,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B39">
         <v>-7.0000000000000007E-2</v>
@@ -4944,7 +4863,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="B40">
         <v>7.3700000000000002E-2</v>
@@ -4967,7 +4886,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B41">
         <v>0.13769999999999999</v>
@@ -4989,9 +4908,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="9" t="s">
-        <v>182</v>
-      </c>
+      <c r="A42" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4999,9 +4916,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5228,27 +5148,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{571F5220-80D8-4F20-8AD7-DC1A6F626947}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78112817-9362-4DB1-B53E-54BAB126672D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5273,9 +5181,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78112817-9362-4DB1-B53E-54BAB126672D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{571F5220-80D8-4F20-8AD7-DC1A6F626947}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>